<commit_message>
Atualização Final do projeto
</commit_message>
<xml_diff>
--- a/INSUMOS.xlsx
+++ b/INSUMOS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\teste\WEBCOREADS2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\teste\WEBCOREBCC2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="69">
   <si>
     <t>GLYCIMAX</t>
   </si>
@@ -228,6 +228,9 @@
   </si>
   <si>
     <t>IMPLEMENTO</t>
+  </si>
+  <si>
+    <t>CodTipo</t>
   </si>
 </sst>
 </file>
@@ -553,20 +556,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C3" sqref="B3:C69"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="127.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="94.44140625" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -576,8 +579,11 @@
       <c r="C1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -588,7 +594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -599,7 +605,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -610,7 +616,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -621,7 +627,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -632,7 +638,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -643,7 +649,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -654,7 +660,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -665,7 +671,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -676,7 +682,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -687,7 +693,7 @@
         <v>73.849999999999994</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -698,7 +704,7 @@
         <v>16.88</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -709,7 +715,7 @@
         <v>126.9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -720,7 +726,7 @@
         <v>88.59</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -731,7 +737,7 @@
         <v>41.17</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>

</xml_diff>